<commit_message>
New values of Goal and ip address
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/SimulinkConfig.xlsx
+++ b/AD-EYE/TA/SimulinkConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,85 +28,85 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Rviz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Sensing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Localization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/FakeLocalization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Detection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/MissionPlanning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/MotionPlanning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Switch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/Ssmp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalPoseX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalPoseY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalPoseZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalOrientX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalOrientY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalOrientZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalOrientW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GoalDistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/GnssPoseSimulink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/PointsRawFloat32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/ImageRaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/ClockFrequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/SimulinkState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/CurrentVelocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/PoseOtherCar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mazda_RX8_Coupe_1/CurrentPose</t>
+    <t xml:space="preserve">Rviz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FakeLocalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MissionPlanning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MotionPlanning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ssmp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalPoseX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalPoseY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalPoseZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalOrientX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalOrientY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalOrientZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalOrientW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoalDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GnssPoseSimulink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PointsRawFloat32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImageRaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClockFrequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimulinkState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CurrentVelocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoseOtherCar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CurrentPose</t>
   </si>
 </sst>
 </file>
@@ -182,11 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,12 +207,12 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A28"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A28 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5991902834008"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -336,7 +332,7 @@
       <c r="A15" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" s="0" t="n">
         <v>0.707</v>
       </c>
     </row>
@@ -360,7 +356,7 @@
       <c r="A18" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" s="0" t="n">
         <v>0.707</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixes, mainly related to folders and experiments names
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/SimulinkConfig.xlsx
+++ b/AD-EYE/TA/SimulinkConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCB37BB-CE3B-4AEA-9860-8B7CCFF3556F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C40194B-5648-47F7-8175-E473FDE9B7CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7884" yWindow="3324" windowWidth="23040" windowHeight="12204" tabRatio="983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="4476" windowWidth="23040" windowHeight="12204" tabRatio="983" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>BlockName</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>CurrentPose</t>
+  </si>
+  <si>
+    <t>percent_reflecting_sfc</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,6 +705,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>